<commit_message>
Nested Logit appears to be working
Both normalizations included in code
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\Ivan\College\2018-2019\Indep Study\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFB35273-2173-49D7-8AC3-3E1FDD7E5BE0}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C0C9D5A-ACD5-4CD8-BEBD-F92D25A095B3}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11715" yWindow="1065" windowWidth="17085" windowHeight="14535" xr2:uid="{F802051B-2499-492A-8A25-373610B69535}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="37">
   <si>
     <t>intercept</t>
   </si>
@@ -143,27 +143,6 @@
   </si>
   <si>
     <t>Characteristics of B</t>
-  </si>
-  <si>
-    <t>Base</t>
-  </si>
-  <si>
-    <t>Store effect A</t>
-  </si>
-  <si>
-    <t>lambda A</t>
-  </si>
-  <si>
-    <t>lambda A + store</t>
-  </si>
-  <si>
-    <t>Horizontal Int Effect</t>
-  </si>
-  <si>
-    <t>Store effects 2</t>
-  </si>
-  <si>
-    <t>Store effects 1</t>
   </si>
 </sst>
 </file>
@@ -706,9 +685,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D70ABDB4-6AEF-4184-89E6-855BD3C5332D}">
   <dimension ref="A1:AP110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AB1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AP26" sqref="AP26"/>
+      <selection pane="bottomLeft" activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -916,137 +895,21 @@
       </c>
     </row>
     <row r="3" spans="1:42" s="7" customFormat="1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="22" t="s">
-        <v>37</v>
-      </c>
-      <c r="B3" s="8">
-        <v>0</v>
-      </c>
-      <c r="C3" s="20">
-        <v>0.5</v>
-      </c>
-      <c r="D3" s="7">
-        <v>1</v>
-      </c>
-      <c r="E3" s="7">
-        <v>1</v>
-      </c>
-      <c r="F3" s="8">
-        <v>0</v>
-      </c>
-      <c r="G3" s="20">
-        <v>0.5</v>
-      </c>
-      <c r="H3" s="7">
-        <v>1</v>
-      </c>
-      <c r="I3" s="7">
-        <v>1</v>
-      </c>
-      <c r="J3" s="8">
-        <v>0</v>
-      </c>
-      <c r="K3" s="7">
-        <v>1</v>
-      </c>
-      <c r="L3" s="7">
-        <v>2</v>
-      </c>
-      <c r="M3" s="8">
-        <v>3</v>
-      </c>
-      <c r="N3" s="7">
-        <v>0.5</v>
-      </c>
-      <c r="O3" s="7">
-        <v>0.5</v>
-      </c>
-      <c r="P3" s="8">
-        <v>0.5</v>
-      </c>
-      <c r="Q3" s="7">
-        <v>1</v>
-      </c>
-      <c r="R3" s="7">
-        <v>0</v>
-      </c>
-      <c r="S3" s="8">
-        <v>1</v>
-      </c>
-      <c r="V3" s="7">
-        <v>3.08</v>
-      </c>
-      <c r="W3" s="7">
-        <v>3.33</v>
-      </c>
-      <c r="X3" s="7">
-        <v>3.08</v>
-      </c>
-      <c r="Y3" s="7">
-        <v>3.33</v>
-      </c>
-      <c r="Z3" s="7">
-        <v>1.52</v>
-      </c>
-      <c r="AA3" s="7">
-        <v>1.77</v>
-      </c>
-      <c r="AB3" s="7">
-        <v>1.52</v>
-      </c>
-      <c r="AC3" s="7">
-        <v>1.77</v>
-      </c>
-      <c r="AD3" s="7">
-        <f t="shared" ref="AD3:AD14" si="0">V3-Z3-$T3</f>
-        <v>1.56</v>
-      </c>
-      <c r="AE3" s="7">
-        <f t="shared" ref="AE3:AE14" si="1">W3-AA3-$T3</f>
-        <v>1.56</v>
-      </c>
-      <c r="AF3" s="7">
-        <f t="shared" ref="AF3:AF14" si="2">X3-AB3-$U3</f>
-        <v>1.56</v>
-      </c>
-      <c r="AG3" s="8">
-        <f t="shared" ref="AG3:AG14" si="3">Y3-AC3-$U3</f>
-        <v>1.56</v>
-      </c>
-      <c r="AH3" s="7">
-        <v>0.157</v>
-      </c>
-      <c r="AI3" s="7">
-        <v>0.20200000000000001</v>
-      </c>
-      <c r="AJ3" s="7">
-        <v>0.157</v>
-      </c>
-      <c r="AK3" s="7">
-        <v>0.20200000000000001</v>
-      </c>
-      <c r="AL3" s="9">
-        <f t="shared" ref="AL3:AL15" si="4">SUM(AH3:AK3)</f>
-        <v>0.71799999999999997</v>
-      </c>
-      <c r="AM3" s="7">
-        <v>0.47799999999999998</v>
-      </c>
-      <c r="AN3" s="7">
-        <v>0.71499999999999997</v>
-      </c>
-      <c r="AO3" s="7">
-        <v>0.56100000000000005</v>
-      </c>
-      <c r="AP3" s="7">
-        <v>0.56100000000000005</v>
-      </c>
+      <c r="A3" s="22"/>
+      <c r="B3" s="8"/>
+      <c r="C3" s="20"/>
+      <c r="F3" s="8"/>
+      <c r="G3" s="20"/>
+      <c r="J3" s="8"/>
+      <c r="M3" s="8"/>
+      <c r="P3" s="8"/>
+      <c r="S3" s="8"/>
+      <c r="AG3" s="8"/>
+      <c r="AL3" s="9"/>
     </row>
     <row r="4" spans="1:42" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="22"/>
-      <c r="B4" s="8">
-        <v>1</v>
-      </c>
+      <c r="B4" s="8"/>
       <c r="C4" s="20"/>
       <c r="F4" s="8"/>
       <c r="G4" s="20"/>
@@ -1054,207 +917,25 @@
       <c r="M4" s="8"/>
       <c r="P4" s="8"/>
       <c r="S4" s="8"/>
-      <c r="V4" s="7">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="W4" s="7">
-        <v>3.64</v>
-      </c>
-      <c r="X4" s="7">
-        <v>3.46</v>
-      </c>
-      <c r="Y4" s="7">
-        <v>3.19</v>
-      </c>
-      <c r="Z4" s="7">
-        <v>0</v>
-      </c>
-      <c r="AA4" s="7">
-        <v>1.44</v>
-      </c>
-      <c r="AB4" s="7">
-        <v>2.04</v>
-      </c>
-      <c r="AC4" s="7">
-        <v>1.77</v>
-      </c>
-      <c r="AD4" s="7">
-        <f t="shared" si="0"/>
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="AE4" s="7">
-        <f t="shared" si="1"/>
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="AF4" s="7">
-        <f t="shared" si="2"/>
-        <v>1.42</v>
-      </c>
-      <c r="AG4" s="8">
-        <f t="shared" si="3"/>
-        <v>1.42</v>
-      </c>
-      <c r="AH4" s="7">
-        <v>0.33</v>
-      </c>
-      <c r="AI4" s="7">
-        <v>0.129</v>
-      </c>
-      <c r="AJ4" s="7">
-        <v>9.3899999999999997E-2</v>
-      </c>
-      <c r="AK4" s="7">
-        <v>0.20200000000000001</v>
-      </c>
-      <c r="AL4" s="9">
-        <f t="shared" si="4"/>
-        <v>0.75490000000000013</v>
-      </c>
-      <c r="AM4" s="7">
-        <v>0.191</v>
-      </c>
-      <c r="AN4" s="7">
-        <v>0.54400000000000004</v>
-      </c>
-      <c r="AO4" s="7">
-        <v>1.01</v>
-      </c>
-      <c r="AP4" s="7">
-        <v>0.42</v>
-      </c>
-    </row>
-    <row r="5" spans="1:42" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="22" t="s">
-        <v>38</v>
-      </c>
-      <c r="B5" s="8">
-        <v>0</v>
-      </c>
-      <c r="C5" s="20">
-        <v>0.5</v>
-      </c>
-      <c r="D5" s="7">
-        <v>1</v>
-      </c>
-      <c r="E5" s="7">
-        <v>1</v>
-      </c>
-      <c r="F5" s="8">
-        <v>1</v>
-      </c>
-      <c r="G5" s="20">
-        <v>0.5</v>
-      </c>
-      <c r="H5" s="7">
-        <v>1</v>
-      </c>
-      <c r="I5" s="7">
-        <v>1</v>
-      </c>
-      <c r="J5" s="8">
-        <v>0</v>
-      </c>
-      <c r="K5" s="7">
-        <v>1</v>
-      </c>
-      <c r="L5" s="7">
-        <v>2</v>
-      </c>
-      <c r="M5" s="8">
-        <v>3</v>
-      </c>
-      <c r="N5" s="7">
-        <v>0.5</v>
-      </c>
-      <c r="O5" s="7">
-        <v>0.5</v>
-      </c>
-      <c r="P5" s="8">
-        <v>0.5</v>
-      </c>
-      <c r="Q5" s="7">
-        <v>1</v>
-      </c>
-      <c r="R5" s="7">
-        <v>0</v>
-      </c>
-      <c r="S5" s="8">
-        <v>1</v>
-      </c>
-      <c r="V5" s="7">
-        <v>3.07</v>
-      </c>
-      <c r="W5" s="7">
-        <v>3.23</v>
-      </c>
-      <c r="X5" s="7">
-        <v>3.52</v>
-      </c>
-      <c r="Y5" s="7">
-        <v>3.33</v>
-      </c>
-      <c r="Z5" s="7">
-        <v>1.57</v>
-      </c>
-      <c r="AA5" s="7">
-        <v>1.73</v>
-      </c>
-      <c r="AB5" s="7">
-        <v>1.8</v>
-      </c>
-      <c r="AC5" s="7">
-        <v>1.61</v>
-      </c>
-      <c r="AD5" s="7">
-        <f t="shared" si="0"/>
-        <v>1.4999999999999998</v>
-      </c>
-      <c r="AE5" s="7">
-        <f t="shared" si="1"/>
-        <v>1.5</v>
-      </c>
-      <c r="AF5" s="7">
-        <f t="shared" si="2"/>
-        <v>1.72</v>
-      </c>
-      <c r="AG5" s="8">
-        <f t="shared" si="3"/>
-        <v>1.72</v>
-      </c>
-      <c r="AH5" s="7">
-        <v>0.13900000000000001</v>
-      </c>
-      <c r="AI5" s="7">
-        <v>0.19600000000000001</v>
-      </c>
-      <c r="AJ5" s="7">
-        <v>0.23100000000000001</v>
-      </c>
-      <c r="AK5" s="7">
-        <v>0.17799999999999999</v>
-      </c>
-      <c r="AL5" s="9">
-        <f t="shared" si="4"/>
-        <v>0.74399999999999999</v>
-      </c>
-      <c r="AM5" s="7">
-        <v>0.65300000000000002</v>
-      </c>
-      <c r="AN5" s="7">
-        <v>0.624</v>
-      </c>
-      <c r="AO5" s="7">
-        <v>0.503</v>
-      </c>
-      <c r="AP5" s="7">
-        <v>0.72</v>
-      </c>
+      <c r="AG4" s="8"/>
+      <c r="AL4" s="9"/>
+    </row>
+    <row r="5" spans="1:42" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="22"/>
+      <c r="B5" s="8"/>
+      <c r="C5" s="20"/>
+      <c r="F5" s="8"/>
+      <c r="G5" s="20"/>
+      <c r="J5" s="8"/>
+      <c r="M5" s="8"/>
+      <c r="P5" s="8"/>
+      <c r="S5" s="8"/>
+      <c r="AG5" s="8"/>
+      <c r="AL5" s="9"/>
     </row>
     <row r="6" spans="1:42" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="22"/>
-      <c r="B6" s="8">
-        <v>1</v>
-      </c>
+      <c r="B6" s="8"/>
       <c r="C6" s="20"/>
       <c r="F6" s="8"/>
       <c r="G6" s="20"/>
@@ -1262,207 +943,25 @@
       <c r="M6" s="8"/>
       <c r="P6" s="8"/>
       <c r="S6" s="8"/>
-      <c r="V6" s="7">
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="W6" s="7">
-        <v>3.7</v>
-      </c>
-      <c r="X6" s="7">
-        <v>3.79</v>
-      </c>
-      <c r="Y6" s="7">
-        <v>3.19</v>
-      </c>
-      <c r="Z6" s="7">
-        <v>0</v>
-      </c>
-      <c r="AA6" s="7">
-        <v>1.4</v>
-      </c>
-      <c r="AB6" s="7">
-        <v>2.21</v>
-      </c>
-      <c r="AC6" s="7">
-        <v>1.6</v>
-      </c>
-      <c r="AD6" s="7">
-        <f t="shared" si="0"/>
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="AE6" s="7">
-        <f t="shared" si="1"/>
-        <v>2.3000000000000003</v>
-      </c>
-      <c r="AF6" s="7">
-        <f t="shared" si="2"/>
-        <v>1.58</v>
-      </c>
-      <c r="AG6" s="8">
-        <f t="shared" si="3"/>
-        <v>1.5899999999999999</v>
-      </c>
-      <c r="AH6" s="7">
-        <v>0.28399999999999997</v>
-      </c>
-      <c r="AI6" s="7">
-        <v>0.115</v>
-      </c>
-      <c r="AJ6" s="7">
-        <v>0.17399999999999999</v>
-      </c>
-      <c r="AK6" s="7">
-        <v>0.19400000000000001</v>
-      </c>
-      <c r="AL6" s="9">
-        <f t="shared" si="4"/>
-        <v>0.7669999999999999</v>
-      </c>
-      <c r="AM6" s="7">
-        <v>0.38500000000000001</v>
-      </c>
-      <c r="AN6" s="7">
-        <v>0.47199999999999998</v>
-      </c>
-      <c r="AO6" s="7">
-        <v>0.92</v>
-      </c>
-      <c r="AP6" s="7">
-        <v>0.58199999999999996</v>
-      </c>
+      <c r="AG6" s="8"/>
+      <c r="AL6" s="9"/>
     </row>
     <row r="7" spans="1:42" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="22" t="s">
-        <v>39</v>
-      </c>
-      <c r="B7" s="8">
-        <v>0</v>
-      </c>
-      <c r="C7" s="20">
-        <v>0.8</v>
-      </c>
-      <c r="D7" s="7">
-        <v>1</v>
-      </c>
-      <c r="E7" s="7">
-        <v>1</v>
-      </c>
-      <c r="F7" s="8">
-        <v>0</v>
-      </c>
-      <c r="G7" s="20">
-        <v>0.5</v>
-      </c>
-      <c r="H7" s="7">
-        <v>1</v>
-      </c>
-      <c r="I7" s="7">
-        <v>1</v>
-      </c>
-      <c r="J7" s="8">
-        <v>0</v>
-      </c>
-      <c r="K7" s="7">
-        <v>1</v>
-      </c>
-      <c r="L7" s="7">
-        <v>2</v>
-      </c>
-      <c r="M7" s="8">
-        <v>3</v>
-      </c>
-      <c r="N7" s="7">
-        <v>0.5</v>
-      </c>
-      <c r="O7" s="7">
-        <v>0.5</v>
-      </c>
-      <c r="P7" s="8">
-        <v>0.5</v>
-      </c>
-      <c r="Q7" s="7">
-        <v>1</v>
-      </c>
-      <c r="R7" s="7">
-        <v>0</v>
-      </c>
-      <c r="S7" s="8">
-        <v>1</v>
-      </c>
-      <c r="V7" s="7">
-        <v>3.45</v>
-      </c>
-      <c r="W7" s="7">
-        <v>3.23</v>
-      </c>
-      <c r="X7" s="7">
-        <v>3.45</v>
-      </c>
-      <c r="Y7" s="7">
-        <v>3.23</v>
-      </c>
-      <c r="Z7" s="7">
-        <v>1.81</v>
-      </c>
-      <c r="AA7" s="7">
-        <v>1.6</v>
-      </c>
-      <c r="AB7" s="7">
-        <v>1.81</v>
-      </c>
-      <c r="AC7" s="7">
-        <v>1.6</v>
-      </c>
-      <c r="AD7" s="7">
-        <f t="shared" si="0"/>
-        <v>1.6400000000000001</v>
-      </c>
-      <c r="AE7" s="7">
-        <f t="shared" si="1"/>
-        <v>1.63</v>
-      </c>
-      <c r="AF7" s="7">
-        <f t="shared" si="2"/>
-        <v>1.6400000000000001</v>
-      </c>
-      <c r="AG7" s="8">
-        <f t="shared" si="3"/>
-        <v>1.63</v>
-      </c>
-      <c r="AH7" s="7">
-        <v>0.21199999999999999</v>
-      </c>
-      <c r="AI7" s="7">
-        <v>0.17599999999999999</v>
-      </c>
-      <c r="AJ7" s="7">
-        <v>0.21199999999999999</v>
-      </c>
-      <c r="AK7" s="7">
-        <v>0.17599999999999999</v>
-      </c>
-      <c r="AL7" s="9">
-        <f t="shared" si="4"/>
-        <v>0.77600000000000002</v>
-      </c>
-      <c r="AM7" s="7">
-        <v>0.76900000000000002</v>
-      </c>
-      <c r="AN7" s="7">
-        <v>0.56299999999999994</v>
-      </c>
-      <c r="AO7" s="7">
-        <v>0.63600000000000001</v>
-      </c>
-      <c r="AP7" s="7">
-        <v>0.63600000000000001</v>
-      </c>
+      <c r="A7" s="22"/>
+      <c r="B7" s="8"/>
+      <c r="C7" s="20"/>
+      <c r="F7" s="8"/>
+      <c r="G7" s="20"/>
+      <c r="J7" s="8"/>
+      <c r="M7" s="8"/>
+      <c r="P7" s="8"/>
+      <c r="S7" s="8"/>
+      <c r="AG7" s="8"/>
+      <c r="AL7" s="9"/>
     </row>
     <row r="8" spans="1:42" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="22"/>
-      <c r="B8" s="8">
-        <v>1</v>
-      </c>
+      <c r="B8" s="8"/>
       <c r="C8" s="20"/>
       <c r="D8" s="7"/>
       <c r="E8" s="7"/>
@@ -1482,207 +981,44 @@
       <c r="S8" s="8"/>
       <c r="T8" s="7"/>
       <c r="U8" s="7"/>
-      <c r="V8" s="7">
-        <v>2.62</v>
-      </c>
-      <c r="W8" s="7">
-        <v>3.89</v>
-      </c>
-      <c r="X8" s="7">
-        <v>3.87</v>
-      </c>
-      <c r="Y8" s="7">
-        <v>3.1</v>
-      </c>
-      <c r="Z8" s="7">
-        <v>0</v>
-      </c>
-      <c r="AA8" s="7">
-        <v>1.26</v>
-      </c>
-      <c r="AB8" s="7">
-        <v>2.44</v>
-      </c>
-      <c r="AC8" s="7">
-        <v>1.67</v>
-      </c>
-      <c r="AD8" s="7">
-        <f t="shared" si="0"/>
-        <v>2.62</v>
-      </c>
-      <c r="AE8" s="7">
-        <f t="shared" si="1"/>
-        <v>2.63</v>
-      </c>
-      <c r="AF8" s="7">
-        <f t="shared" si="2"/>
-        <v>1.4300000000000002</v>
-      </c>
-      <c r="AG8" s="8">
-        <f t="shared" si="3"/>
-        <v>1.4300000000000002</v>
-      </c>
-      <c r="AH8" s="7">
-        <v>0.42399999999999999</v>
-      </c>
-      <c r="AI8" s="7">
-        <v>8.0500000000000002E-2</v>
-      </c>
-      <c r="AJ8" s="7">
-        <v>0.123</v>
-      </c>
-      <c r="AK8" s="7">
-        <v>0.17699999999999999</v>
-      </c>
-      <c r="AL8" s="9">
-        <f t="shared" si="4"/>
-        <v>0.80449999999999999</v>
-      </c>
-      <c r="AM8" s="7">
-        <v>0.29899999999999999</v>
-      </c>
-      <c r="AN8" s="7">
-        <v>0.39700000000000002</v>
-      </c>
-      <c r="AO8" s="7">
-        <v>1.32</v>
-      </c>
-      <c r="AP8" s="7">
-        <v>0.42799999999999999</v>
-      </c>
+      <c r="V8" s="7"/>
+      <c r="W8" s="7"/>
+      <c r="X8" s="7"/>
+      <c r="Y8" s="7"/>
+      <c r="Z8" s="7"/>
+      <c r="AA8" s="7"/>
+      <c r="AB8" s="7"/>
+      <c r="AC8" s="7"/>
+      <c r="AD8" s="7"/>
+      <c r="AE8" s="7"/>
+      <c r="AF8" s="7"/>
+      <c r="AG8" s="8"/>
+      <c r="AH8" s="7"/>
+      <c r="AI8" s="7"/>
+      <c r="AJ8" s="7"/>
+      <c r="AK8" s="7"/>
+      <c r="AL8" s="9"/>
+      <c r="AM8" s="7"/>
+      <c r="AN8" s="7"/>
+      <c r="AO8" s="7"/>
+      <c r="AP8" s="7"/>
     </row>
     <row r="9" spans="1:42" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="22" t="s">
-        <v>39</v>
-      </c>
-      <c r="B9" s="8">
-        <v>0</v>
-      </c>
-      <c r="C9" s="20">
-        <v>0.1</v>
-      </c>
-      <c r="D9" s="7">
-        <v>1</v>
-      </c>
-      <c r="E9" s="7">
-        <v>1</v>
-      </c>
-      <c r="F9" s="8">
-        <v>0</v>
-      </c>
-      <c r="G9" s="20">
-        <v>0.5</v>
-      </c>
-      <c r="H9" s="7">
-        <v>1</v>
-      </c>
-      <c r="I9" s="7">
-        <v>1</v>
-      </c>
-      <c r="J9" s="8">
-        <v>0</v>
-      </c>
-      <c r="K9" s="7">
-        <v>1</v>
-      </c>
-      <c r="L9" s="7">
-        <v>2</v>
-      </c>
-      <c r="M9" s="8">
-        <v>3</v>
-      </c>
-      <c r="N9" s="7">
-        <v>0.5</v>
-      </c>
-      <c r="O9" s="7">
-        <v>0.5</v>
-      </c>
-      <c r="P9" s="8">
-        <v>0.5</v>
-      </c>
-      <c r="Q9" s="7">
-        <v>1</v>
-      </c>
-      <c r="R9" s="7">
-        <v>0</v>
-      </c>
-      <c r="S9" s="8">
-        <v>1</v>
-      </c>
-      <c r="V9" s="7">
-        <v>2.71</v>
-      </c>
-      <c r="W9" s="7">
-        <v>3.48</v>
-      </c>
-      <c r="X9" s="7">
-        <v>2.71</v>
-      </c>
-      <c r="Y9" s="7">
-        <v>3.48</v>
-      </c>
-      <c r="Z9" s="7">
-        <v>1.25</v>
-      </c>
-      <c r="AA9" s="7">
-        <v>2.02</v>
-      </c>
-      <c r="AB9" s="7">
-        <v>1.25</v>
-      </c>
-      <c r="AC9" s="7">
-        <v>2.02</v>
-      </c>
-      <c r="AD9" s="7">
-        <f t="shared" si="0"/>
-        <v>1.46</v>
-      </c>
-      <c r="AE9" s="7">
-        <f t="shared" si="1"/>
-        <v>1.46</v>
-      </c>
-      <c r="AF9" s="7">
-        <f t="shared" si="2"/>
-        <v>1.46</v>
-      </c>
-      <c r="AG9" s="8">
-        <f t="shared" si="3"/>
-        <v>1.46</v>
-      </c>
-      <c r="AH9" s="7">
-        <v>8.9399999999999993E-2</v>
-      </c>
-      <c r="AI9" s="7">
-        <v>0.22700000000000001</v>
-      </c>
-      <c r="AJ9" s="7">
-        <v>8.9399999999999993E-2</v>
-      </c>
-      <c r="AK9" s="7">
-        <v>0.22700000000000001</v>
-      </c>
-      <c r="AL9" s="9">
-        <f t="shared" si="4"/>
-        <v>0.63280000000000003</v>
-      </c>
-      <c r="AM9" s="7">
-        <v>0.224</v>
-      </c>
-      <c r="AN9" s="7">
-        <v>0.91700000000000004</v>
-      </c>
-      <c r="AO9" s="7">
-        <v>0.46200000000000002</v>
-      </c>
-      <c r="AP9" s="7">
-        <v>0.46200000000000002</v>
-      </c>
+      <c r="A9" s="22"/>
+      <c r="B9" s="8"/>
+      <c r="C9" s="20"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="20"/>
+      <c r="J9" s="8"/>
+      <c r="M9" s="8"/>
+      <c r="P9" s="8"/>
+      <c r="S9" s="8"/>
+      <c r="AG9" s="8"/>
+      <c r="AL9" s="9"/>
     </row>
     <row r="10" spans="1:42" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="22"/>
-      <c r="B10" s="8">
-        <v>1</v>
-      </c>
+      <c r="B10" s="8"/>
       <c r="C10" s="20"/>
       <c r="D10" s="7"/>
       <c r="E10" s="7"/>
@@ -1702,207 +1038,44 @@
       <c r="S10" s="8"/>
       <c r="T10" s="7"/>
       <c r="U10" s="7"/>
-      <c r="V10" s="7">
-        <v>1.79</v>
-      </c>
-      <c r="W10" s="7">
-        <v>3.54</v>
-      </c>
-      <c r="X10" s="7">
-        <v>3.05</v>
-      </c>
-      <c r="Y10" s="7">
-        <v>3.36</v>
-      </c>
-      <c r="Z10" s="7">
-        <v>0</v>
-      </c>
-      <c r="AA10" s="7">
-        <v>1.75</v>
-      </c>
-      <c r="AB10" s="7">
-        <v>1.66</v>
-      </c>
-      <c r="AC10" s="7">
-        <v>1.96</v>
-      </c>
-      <c r="AD10" s="7">
-        <f t="shared" si="0"/>
-        <v>1.79</v>
-      </c>
-      <c r="AE10" s="7">
-        <f t="shared" si="1"/>
-        <v>1.79</v>
-      </c>
-      <c r="AF10" s="7">
-        <f t="shared" si="2"/>
-        <v>1.39</v>
-      </c>
-      <c r="AG10" s="8">
-        <f t="shared" si="3"/>
-        <v>1.4</v>
-      </c>
-      <c r="AH10" s="13">
-        <v>0.2</v>
-      </c>
-      <c r="AI10" s="13">
-        <v>0.19</v>
-      </c>
-      <c r="AJ10" s="13">
-        <v>5.6500000000000002E-2</v>
-      </c>
-      <c r="AK10" s="13">
-        <v>0.22800000000000001</v>
-      </c>
-      <c r="AL10" s="9">
-        <f t="shared" si="4"/>
-        <v>0.67449999999999999</v>
-      </c>
-      <c r="AM10" s="7">
-        <v>9.3600000000000003E-2</v>
-      </c>
-      <c r="AN10" s="7">
-        <v>0.77900000000000003</v>
-      </c>
-      <c r="AO10" s="7">
-        <v>0.69699999999999995</v>
-      </c>
-      <c r="AP10" s="7">
-        <v>0.39700000000000002</v>
-      </c>
-    </row>
-    <row r="11" spans="1:42" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="22" t="s">
-        <v>40</v>
-      </c>
-      <c r="B11" s="8">
-        <v>0</v>
-      </c>
-      <c r="C11" s="20">
-        <v>0.8</v>
-      </c>
-      <c r="D11" s="7">
-        <v>1</v>
-      </c>
-      <c r="E11" s="7">
-        <v>1</v>
-      </c>
-      <c r="F11" s="8">
-        <v>1</v>
-      </c>
-      <c r="G11" s="20">
-        <v>0.5</v>
-      </c>
-      <c r="H11" s="7">
-        <v>1</v>
-      </c>
-      <c r="I11" s="7">
-        <v>1</v>
-      </c>
-      <c r="J11" s="8">
-        <v>0</v>
-      </c>
-      <c r="K11" s="7">
-        <v>1</v>
-      </c>
-      <c r="L11" s="7">
-        <v>2</v>
-      </c>
-      <c r="M11" s="8">
-        <v>3</v>
-      </c>
-      <c r="N11" s="7">
-        <v>0.5</v>
-      </c>
-      <c r="O11" s="7">
-        <v>0.5</v>
-      </c>
-      <c r="P11" s="8">
-        <v>0.5</v>
-      </c>
-      <c r="Q11" s="7">
-        <v>1</v>
-      </c>
-      <c r="R11" s="7">
-        <v>0</v>
-      </c>
-      <c r="S11" s="8">
-        <v>1</v>
-      </c>
-      <c r="V11" s="7">
-        <v>3.44</v>
-      </c>
-      <c r="W11" s="7">
-        <v>3.13</v>
-      </c>
-      <c r="X11" s="7">
-        <v>3.98</v>
-      </c>
-      <c r="Y11" s="7">
-        <v>3.26</v>
-      </c>
-      <c r="Z11" s="7">
-        <v>1.88</v>
-      </c>
-      <c r="AA11" s="7">
-        <v>1.57</v>
-      </c>
-      <c r="AB11" s="7">
-        <v>2.1800000000000002</v>
-      </c>
-      <c r="AC11" s="7">
-        <v>1.46</v>
-      </c>
-      <c r="AD11" s="7">
-        <f t="shared" si="0"/>
-        <v>1.56</v>
-      </c>
-      <c r="AE11" s="7">
-        <f t="shared" si="1"/>
-        <v>1.5599999999999998</v>
-      </c>
-      <c r="AF11" s="7">
-        <f t="shared" si="2"/>
-        <v>1.7999999999999998</v>
-      </c>
-      <c r="AG11" s="8">
-        <f t="shared" si="3"/>
-        <v>1.7999999999999998</v>
-      </c>
-      <c r="AH11" s="7">
-        <v>0.188</v>
-      </c>
-      <c r="AI11" s="7">
-        <v>0.17100000000000001</v>
-      </c>
-      <c r="AJ11" s="7">
-        <v>0.29599999999999999</v>
-      </c>
-      <c r="AK11" s="7">
-        <v>0.15</v>
-      </c>
-      <c r="AL11" s="9">
-        <f t="shared" si="4"/>
-        <v>0.80500000000000005</v>
-      </c>
-      <c r="AM11" s="7">
-        <v>0.998</v>
-      </c>
-      <c r="AN11" s="7">
-        <v>0.48799999999999999</v>
-      </c>
-      <c r="AO11" s="7">
-        <v>0.56000000000000005</v>
-      </c>
-      <c r="AP11" s="7">
-        <v>0.80400000000000005</v>
-      </c>
+      <c r="V10" s="7"/>
+      <c r="W10" s="7"/>
+      <c r="X10" s="7"/>
+      <c r="Y10" s="7"/>
+      <c r="Z10" s="7"/>
+      <c r="AA10" s="7"/>
+      <c r="AB10" s="7"/>
+      <c r="AC10" s="7"/>
+      <c r="AD10" s="7"/>
+      <c r="AE10" s="7"/>
+      <c r="AF10" s="7"/>
+      <c r="AG10" s="8"/>
+      <c r="AH10" s="13"/>
+      <c r="AI10" s="13"/>
+      <c r="AJ10" s="13"/>
+      <c r="AK10" s="13"/>
+      <c r="AL10" s="9"/>
+      <c r="AM10" s="7"/>
+      <c r="AN10" s="7"/>
+      <c r="AO10" s="7"/>
+      <c r="AP10" s="7"/>
+    </row>
+    <row r="11" spans="1:42" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="22"/>
+      <c r="B11" s="8"/>
+      <c r="C11" s="20"/>
+      <c r="F11" s="8"/>
+      <c r="G11" s="20"/>
+      <c r="J11" s="8"/>
+      <c r="M11" s="8"/>
+      <c r="P11" s="8"/>
+      <c r="S11" s="8"/>
+      <c r="AG11" s="8"/>
+      <c r="AL11" s="9"/>
     </row>
     <row r="12" spans="1:42" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="22"/>
-      <c r="B12" s="8">
-        <v>1</v>
-      </c>
+      <c r="B12" s="8"/>
       <c r="C12" s="20"/>
       <c r="D12" s="7"/>
       <c r="E12" s="7"/>
@@ -1922,207 +1095,44 @@
       <c r="S12" s="8"/>
       <c r="T12" s="7"/>
       <c r="U12" s="7"/>
-      <c r="V12" s="7">
-        <v>2.75</v>
-      </c>
-      <c r="W12" s="7">
-        <v>3.99</v>
-      </c>
-      <c r="X12" s="7">
-        <v>4.2699999999999996</v>
-      </c>
-      <c r="Y12" s="7">
-        <v>3.12</v>
-      </c>
-      <c r="Z12" s="7">
-        <v>0</v>
-      </c>
-      <c r="AA12" s="7">
-        <v>1.24</v>
-      </c>
-      <c r="AB12" s="7">
-        <v>2.66</v>
-      </c>
-      <c r="AC12" s="7">
-        <v>1.51</v>
-      </c>
-      <c r="AD12" s="7">
-        <f t="shared" si="0"/>
-        <v>2.75</v>
-      </c>
-      <c r="AE12" s="7">
-        <f t="shared" si="1"/>
-        <v>2.75</v>
-      </c>
-      <c r="AF12" s="7">
-        <f t="shared" si="2"/>
-        <v>1.6099999999999994</v>
-      </c>
-      <c r="AG12" s="8">
-        <f t="shared" si="3"/>
-        <v>1.61</v>
-      </c>
-      <c r="AH12" s="7">
-        <v>0.36</v>
-      </c>
-      <c r="AI12" s="7">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="AJ12" s="7">
-        <v>0.215</v>
-      </c>
-      <c r="AK12" s="7">
-        <v>0.16700000000000001</v>
-      </c>
-      <c r="AL12" s="9">
-        <f t="shared" si="4"/>
-        <v>0.81200000000000006</v>
-      </c>
-      <c r="AM12" s="7">
-        <v>0.56999999999999995</v>
-      </c>
-      <c r="AN12" s="7">
-        <v>0.33800000000000002</v>
-      </c>
-      <c r="AO12" s="7">
-        <v>1.18</v>
-      </c>
-      <c r="AP12" s="7">
-        <v>0.61599999999999999</v>
-      </c>
-    </row>
-    <row r="13" spans="1:42" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="22" t="s">
-        <v>41</v>
-      </c>
-      <c r="B13" s="8">
-        <v>0</v>
-      </c>
-      <c r="C13" s="20">
-        <v>0.9</v>
-      </c>
-      <c r="D13" s="7">
-        <v>3.2</v>
-      </c>
-      <c r="E13" s="7">
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="F13" s="8">
-        <v>2</v>
-      </c>
-      <c r="G13" s="20">
-        <v>0.2</v>
-      </c>
-      <c r="H13" s="7">
-        <v>3</v>
-      </c>
-      <c r="I13" s="7">
-        <v>2</v>
-      </c>
-      <c r="J13" s="8">
-        <v>0</v>
-      </c>
-      <c r="K13" s="7">
-        <v>2</v>
-      </c>
-      <c r="L13" s="7">
-        <v>2</v>
-      </c>
-      <c r="M13" s="8">
-        <v>2</v>
-      </c>
-      <c r="N13" s="7">
-        <v>2.5</v>
-      </c>
-      <c r="O13" s="7">
-        <v>2</v>
-      </c>
-      <c r="P13" s="8">
-        <v>2</v>
-      </c>
-      <c r="Q13" s="7">
-        <v>-1</v>
-      </c>
-      <c r="R13" s="7">
-        <v>-1</v>
-      </c>
-      <c r="S13" s="8">
-        <v>-1</v>
-      </c>
-      <c r="V13" s="7">
-        <v>3.11</v>
-      </c>
-      <c r="W13" s="7">
-        <v>1.2</v>
-      </c>
-      <c r="X13" s="7">
-        <v>3.52</v>
-      </c>
-      <c r="Y13" s="7">
-        <v>1.31</v>
-      </c>
-      <c r="Z13" s="7">
-        <v>2.68</v>
-      </c>
-      <c r="AA13" s="7">
-        <v>0.51900000000000002</v>
-      </c>
-      <c r="AB13" s="7">
-        <v>2.98</v>
-      </c>
-      <c r="AC13" s="7">
-        <v>0.50700000000000001</v>
-      </c>
-      <c r="AD13" s="7">
-        <f t="shared" si="0"/>
-        <v>0.42999999999999972</v>
-      </c>
-      <c r="AE13" s="7">
-        <f t="shared" si="1"/>
-        <v>0.68099999999999994</v>
-      </c>
-      <c r="AF13" s="7">
-        <f t="shared" si="2"/>
-        <v>0.54</v>
-      </c>
-      <c r="AG13" s="8">
-        <f t="shared" si="3"/>
-        <v>0.80300000000000005</v>
-      </c>
-      <c r="AH13" s="7">
-        <v>0.38800000000000001</v>
-      </c>
-      <c r="AI13" s="7">
-        <v>2.4500000000000001E-2</v>
-      </c>
-      <c r="AJ13" s="7">
-        <v>0.52300000000000002</v>
-      </c>
-      <c r="AK13" s="7">
-        <v>1.9800000000000002E-2</v>
-      </c>
-      <c r="AL13" s="9">
-        <f t="shared" si="4"/>
-        <v>0.95530000000000004</v>
-      </c>
-      <c r="AM13" s="7">
-        <v>2.6</v>
-      </c>
-      <c r="AN13" s="7">
-        <v>2.2700000000000001E-2</v>
-      </c>
-      <c r="AO13" s="7">
-        <v>0.182</v>
-      </c>
-      <c r="AP13" s="7">
-        <v>0.30099999999999999</v>
-      </c>
+      <c r="V12" s="7"/>
+      <c r="W12" s="7"/>
+      <c r="X12" s="7"/>
+      <c r="Y12" s="7"/>
+      <c r="Z12" s="7"/>
+      <c r="AA12" s="7"/>
+      <c r="AB12" s="7"/>
+      <c r="AC12" s="7"/>
+      <c r="AD12" s="7"/>
+      <c r="AE12" s="7"/>
+      <c r="AF12" s="7"/>
+      <c r="AG12" s="8"/>
+      <c r="AH12" s="7"/>
+      <c r="AI12" s="7"/>
+      <c r="AJ12" s="7"/>
+      <c r="AK12" s="7"/>
+      <c r="AL12" s="9"/>
+      <c r="AM12" s="7"/>
+      <c r="AN12" s="7"/>
+      <c r="AO12" s="7"/>
+      <c r="AP12" s="7"/>
+    </row>
+    <row r="13" spans="1:42" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="22"/>
+      <c r="B13" s="8"/>
+      <c r="C13" s="20"/>
+      <c r="F13" s="8"/>
+      <c r="G13" s="20"/>
+      <c r="J13" s="8"/>
+      <c r="M13" s="8"/>
+      <c r="P13" s="8"/>
+      <c r="S13" s="8"/>
+      <c r="AG13" s="8"/>
+      <c r="AL13" s="9"/>
     </row>
     <row r="14" spans="1:42" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="22"/>
-      <c r="B14" s="8">
-        <v>1</v>
-      </c>
+      <c r="B14" s="8"/>
       <c r="C14" s="20"/>
       <c r="D14" s="7"/>
       <c r="E14" s="7"/>
@@ -2142,207 +1152,44 @@
       <c r="S14" s="8"/>
       <c r="T14" s="7"/>
       <c r="U14" s="7"/>
-      <c r="V14" s="7">
-        <v>3.13</v>
-      </c>
-      <c r="W14" s="7">
-        <v>4.79</v>
-      </c>
-      <c r="X14" s="7">
-        <v>3.67</v>
-      </c>
-      <c r="Y14" s="7">
-        <v>1.31</v>
-      </c>
-      <c r="Z14" s="7">
-        <v>0</v>
-      </c>
-      <c r="AA14" s="7">
-        <v>1.41</v>
-      </c>
-      <c r="AB14" s="7">
-        <v>3.23</v>
-      </c>
-      <c r="AC14" s="7">
-        <v>0.60899999999999999</v>
-      </c>
-      <c r="AD14" s="7">
-        <f t="shared" si="0"/>
-        <v>3.13</v>
-      </c>
-      <c r="AE14" s="7">
-        <f t="shared" si="1"/>
-        <v>3.38</v>
-      </c>
-      <c r="AF14" s="7">
-        <f t="shared" si="2"/>
-        <v>0.43999999999999995</v>
-      </c>
-      <c r="AG14" s="8">
-        <f t="shared" si="3"/>
-        <v>0.70100000000000007</v>
-      </c>
-      <c r="AH14" s="7">
-        <v>0.505</v>
-      </c>
-      <c r="AI14" s="11">
-        <v>2.62E-5</v>
-      </c>
-      <c r="AJ14" s="7">
-        <v>0.40400000000000003</v>
-      </c>
-      <c r="AK14" s="7">
-        <v>2.9700000000000001E-2</v>
-      </c>
-      <c r="AL14" s="9">
-        <f t="shared" si="4"/>
-        <v>0.93872619999999996</v>
-      </c>
-      <c r="AM14" s="7">
-        <v>1.3</v>
-      </c>
-      <c r="AN14" s="7">
-        <v>1.7000000000000001E-2</v>
-      </c>
-      <c r="AO14" s="7">
-        <v>1.58</v>
-      </c>
-      <c r="AP14" s="7">
-        <v>0.19800000000000001</v>
-      </c>
-    </row>
-    <row r="15" spans="1:42" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="22" t="s">
-        <v>41</v>
-      </c>
-      <c r="B15" s="8">
-        <v>0</v>
-      </c>
-      <c r="C15" s="20">
-        <v>0.09</v>
-      </c>
-      <c r="D15" s="7">
-        <v>2</v>
-      </c>
-      <c r="E15" s="7">
-        <v>3</v>
-      </c>
-      <c r="F15" s="8">
-        <v>4</v>
-      </c>
-      <c r="G15" s="20">
-        <v>0.2</v>
-      </c>
-      <c r="H15" s="7">
-        <v>-1</v>
-      </c>
-      <c r="I15" s="7">
-        <v>1</v>
-      </c>
-      <c r="J15" s="8">
-        <v>1</v>
-      </c>
-      <c r="K15" s="7">
-        <v>2</v>
-      </c>
-      <c r="L15" s="7">
-        <v>2</v>
-      </c>
-      <c r="M15" s="8">
-        <v>2</v>
-      </c>
-      <c r="N15" s="7">
-        <v>2</v>
-      </c>
-      <c r="O15" s="7">
-        <v>3</v>
-      </c>
-      <c r="P15" s="8">
-        <v>2</v>
-      </c>
-      <c r="Q15" s="7">
-        <v>1</v>
-      </c>
-      <c r="R15" s="7">
-        <v>0.5</v>
-      </c>
-      <c r="S15" s="8">
-        <v>1</v>
-      </c>
-      <c r="V15" s="7">
-        <v>1.24</v>
-      </c>
-      <c r="W15" s="7">
-        <v>2.21</v>
-      </c>
-      <c r="X15" s="7">
-        <v>2.2200000000000002</v>
-      </c>
-      <c r="Y15" s="7">
-        <v>2.4900000000000002</v>
-      </c>
-      <c r="Z15" s="7">
-        <v>0.80200000000000005</v>
-      </c>
-      <c r="AA15" s="7">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="AB15" s="7">
-        <v>1.4</v>
-      </c>
-      <c r="AC15" s="7">
-        <v>1.01</v>
-      </c>
-      <c r="AD15" s="7">
-        <f t="shared" ref="AD15:AD16" si="5">V15-Z15-$T15</f>
-        <v>0.43799999999999994</v>
-      </c>
-      <c r="AE15" s="7">
-        <f t="shared" ref="AE15:AE16" si="6">W15-AA15-$T15</f>
-        <v>1.1099999999999999</v>
-      </c>
-      <c r="AF15" s="7">
-        <f t="shared" ref="AF15:AF16" si="7">X15-AB15-$U15</f>
-        <v>0.82000000000000028</v>
-      </c>
-      <c r="AG15" s="8">
-        <f t="shared" ref="AG15:AG16" si="8">Y15-AC15-$U15</f>
-        <v>1.4800000000000002</v>
-      </c>
-      <c r="AH15" s="7">
-        <v>0.16600000000000001</v>
-      </c>
-      <c r="AI15" s="7">
-        <v>2.8899999999999999E-2</v>
-      </c>
-      <c r="AJ15" s="7">
-        <v>0.48199999999999998</v>
-      </c>
-      <c r="AK15" s="7">
-        <v>5.9299999999999999E-2</v>
-      </c>
-      <c r="AL15" s="9">
-        <f t="shared" ref="AL15:AL16" si="9">SUM(AH15:AK15)</f>
-        <v>0.73620000000000008</v>
-      </c>
-      <c r="AM15" s="7">
-        <v>0.81100000000000005</v>
-      </c>
-      <c r="AN15" s="7">
-        <v>9.1800000000000007E-2</v>
-      </c>
-      <c r="AO15" s="7">
-        <v>0.105</v>
-      </c>
-      <c r="AP15" s="7">
-        <v>0.48</v>
-      </c>
+      <c r="V14" s="7"/>
+      <c r="W14" s="7"/>
+      <c r="X14" s="7"/>
+      <c r="Y14" s="7"/>
+      <c r="Z14" s="7"/>
+      <c r="AA14" s="7"/>
+      <c r="AB14" s="7"/>
+      <c r="AC14" s="7"/>
+      <c r="AD14" s="7"/>
+      <c r="AE14" s="7"/>
+      <c r="AF14" s="7"/>
+      <c r="AG14" s="8"/>
+      <c r="AH14" s="7"/>
+      <c r="AI14" s="11"/>
+      <c r="AJ14" s="7"/>
+      <c r="AK14" s="7"/>
+      <c r="AL14" s="9"/>
+      <c r="AM14" s="7"/>
+      <c r="AN14" s="7"/>
+      <c r="AO14" s="7"/>
+      <c r="AP14" s="7"/>
+    </row>
+    <row r="15" spans="1:42" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="22"/>
+      <c r="B15" s="8"/>
+      <c r="C15" s="20"/>
+      <c r="F15" s="8"/>
+      <c r="G15" s="20"/>
+      <c r="J15" s="8"/>
+      <c r="M15" s="8"/>
+      <c r="P15" s="8"/>
+      <c r="S15" s="8"/>
+      <c r="AG15" s="8"/>
+      <c r="AL15" s="9"/>
     </row>
     <row r="16" spans="1:42" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="22"/>
-      <c r="B16" s="8">
-        <v>1</v>
-      </c>
+      <c r="B16" s="8"/>
       <c r="C16" s="20"/>
       <c r="D16" s="7"/>
       <c r="E16" s="7"/>
@@ -2362,207 +1209,44 @@
       <c r="S16" s="8"/>
       <c r="T16" s="7"/>
       <c r="U16" s="7"/>
-      <c r="V16" s="7">
-        <v>1.26</v>
-      </c>
-      <c r="W16" s="7">
-        <v>3</v>
-      </c>
-      <c r="X16" s="7">
-        <v>2.2799999999999998</v>
-      </c>
-      <c r="Y16" s="7">
-        <v>2.5299999999999998</v>
-      </c>
-      <c r="Z16" s="7">
-        <v>0</v>
-      </c>
-      <c r="AA16" s="7">
-        <v>1.08</v>
-      </c>
-      <c r="AB16" s="7">
-        <v>1.5</v>
-      </c>
-      <c r="AC16" s="7">
-        <v>1.0900000000000001</v>
-      </c>
-      <c r="AD16" s="7">
-        <f t="shared" si="5"/>
-        <v>1.26</v>
-      </c>
-      <c r="AE16" s="7">
-        <f t="shared" si="6"/>
-        <v>1.92</v>
-      </c>
-      <c r="AF16" s="7">
-        <f t="shared" si="7"/>
-        <v>0.7799999999999998</v>
-      </c>
-      <c r="AG16" s="8">
-        <f t="shared" si="8"/>
-        <v>1.4399999999999997</v>
-      </c>
-      <c r="AH16" s="7">
-        <v>0.17499999999999999</v>
-      </c>
-      <c r="AI16" s="27">
-        <v>1.46E-2</v>
-      </c>
-      <c r="AJ16" s="7">
-        <v>0.45200000000000001</v>
-      </c>
-      <c r="AK16" s="7">
-        <v>6.3799999999999996E-2</v>
-      </c>
-      <c r="AL16" s="9">
-        <f t="shared" si="9"/>
-        <v>0.70539999999999992</v>
-      </c>
-      <c r="AM16" s="7">
-        <v>0.67900000000000005</v>
-      </c>
-      <c r="AN16" s="7">
-        <v>8.5000000000000006E-2</v>
-      </c>
-      <c r="AO16" s="7">
-        <v>0.249</v>
-      </c>
-      <c r="AP16" s="7">
-        <v>0.44400000000000001</v>
-      </c>
-    </row>
-    <row r="17" spans="1:42" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="22" t="s">
-        <v>41</v>
-      </c>
-      <c r="B17" s="8">
-        <v>0</v>
-      </c>
-      <c r="C17" s="20">
-        <v>0.09</v>
-      </c>
-      <c r="D17" s="7">
-        <v>3</v>
-      </c>
-      <c r="E17" s="7">
-        <v>2</v>
-      </c>
-      <c r="F17" s="8">
-        <v>3.5</v>
-      </c>
-      <c r="G17" s="20">
-        <v>0.2</v>
-      </c>
-      <c r="H17" s="7">
-        <v>1</v>
-      </c>
-      <c r="I17" s="7">
-        <v>1</v>
-      </c>
-      <c r="J17" s="8">
-        <v>1</v>
-      </c>
-      <c r="K17" s="7">
-        <v>2</v>
-      </c>
-      <c r="L17" s="7">
-        <v>2</v>
-      </c>
-      <c r="M17" s="8">
-        <v>2</v>
-      </c>
-      <c r="N17" s="7">
-        <v>2</v>
-      </c>
-      <c r="O17" s="7">
-        <v>3</v>
-      </c>
-      <c r="P17" s="8">
-        <v>2</v>
-      </c>
-      <c r="Q17" s="7">
-        <v>1</v>
-      </c>
-      <c r="R17" s="7">
-        <v>0.5</v>
-      </c>
-      <c r="S17" s="8">
-        <v>1</v>
-      </c>
-      <c r="V17" s="7">
-        <v>1.9</v>
-      </c>
-      <c r="W17" s="7">
-        <v>2.5299999999999998</v>
-      </c>
-      <c r="X17" s="7">
-        <v>3.24</v>
-      </c>
-      <c r="Y17" s="7">
-        <v>3.01</v>
-      </c>
-      <c r="Z17" s="7">
-        <v>1.1499999999999999</v>
-      </c>
-      <c r="AA17" s="7">
-        <v>1.28</v>
-      </c>
-      <c r="AB17" s="7">
-        <v>1.86</v>
-      </c>
-      <c r="AC17" s="7">
-        <v>1.1299999999999999</v>
-      </c>
-      <c r="AD17" s="7">
-        <f t="shared" ref="AD17:AD18" si="10">V17-Z17-$T17</f>
-        <v>0.75</v>
-      </c>
-      <c r="AE17" s="7">
-        <f t="shared" ref="AE17:AE18" si="11">W17-AA17-$T17</f>
-        <v>1.2499999999999998</v>
-      </c>
-      <c r="AF17" s="7">
-        <f t="shared" ref="AF17:AF18" si="12">X17-AB17-$U17</f>
-        <v>1.3800000000000001</v>
-      </c>
-      <c r="AG17" s="8">
-        <f t="shared" ref="AG17:AG18" si="13">Y17-AC17-$U17</f>
-        <v>1.88</v>
-      </c>
-      <c r="AH17" s="7">
-        <v>0.20399999999999999</v>
-      </c>
-      <c r="AI17" s="7">
-        <v>7.5700000000000003E-2</v>
-      </c>
-      <c r="AJ17" s="7">
-        <v>0.46500000000000002</v>
-      </c>
-      <c r="AK17" s="7">
-        <v>0.127</v>
-      </c>
-      <c r="AL17" s="9">
-        <f t="shared" ref="AL17:AL18" si="14">SUM(AH17:AK17)</f>
-        <v>0.87170000000000003</v>
-      </c>
-      <c r="AM17" s="7">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="AN17" s="7">
-        <v>0.24099999999999999</v>
-      </c>
-      <c r="AO17" s="7">
-        <v>0.247</v>
-      </c>
-      <c r="AP17" s="7">
-        <v>0.88100000000000001</v>
-      </c>
+      <c r="V16" s="7"/>
+      <c r="W16" s="7"/>
+      <c r="X16" s="7"/>
+      <c r="Y16" s="7"/>
+      <c r="Z16" s="7"/>
+      <c r="AA16" s="7"/>
+      <c r="AB16" s="7"/>
+      <c r="AC16" s="7"/>
+      <c r="AD16" s="7"/>
+      <c r="AE16" s="7"/>
+      <c r="AF16" s="7"/>
+      <c r="AG16" s="8"/>
+      <c r="AH16" s="7"/>
+      <c r="AI16" s="27"/>
+      <c r="AJ16" s="7"/>
+      <c r="AK16" s="7"/>
+      <c r="AL16" s="9"/>
+      <c r="AM16" s="7"/>
+      <c r="AN16" s="7"/>
+      <c r="AO16" s="7"/>
+      <c r="AP16" s="7"/>
+    </row>
+    <row r="17" spans="1:42" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="22"/>
+      <c r="B17" s="8"/>
+      <c r="C17" s="20"/>
+      <c r="F17" s="8"/>
+      <c r="G17" s="20"/>
+      <c r="J17" s="8"/>
+      <c r="M17" s="8"/>
+      <c r="P17" s="8"/>
+      <c r="S17" s="8"/>
+      <c r="AG17" s="8"/>
+      <c r="AL17" s="9"/>
     </row>
     <row r="18" spans="1:42" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="22"/>
-      <c r="B18" s="8">
-        <v>1</v>
-      </c>
+      <c r="B18" s="8"/>
       <c r="C18" s="20"/>
       <c r="D18" s="7"/>
       <c r="E18" s="7"/>
@@ -2582,207 +1266,44 @@
       <c r="S18" s="8"/>
       <c r="T18" s="7"/>
       <c r="U18" s="7"/>
-      <c r="V18" s="7">
-        <v>1.93</v>
-      </c>
-      <c r="W18" s="7">
-        <v>3.57</v>
-      </c>
-      <c r="X18" s="7">
-        <v>3.41</v>
-      </c>
-      <c r="Y18" s="7">
-        <v>3.14</v>
-      </c>
-      <c r="Z18" s="7">
-        <v>0</v>
-      </c>
-      <c r="AA18" s="7">
-        <v>1.1299999999999999</v>
-      </c>
-      <c r="AB18" s="7">
-        <v>2.12</v>
-      </c>
-      <c r="AC18" s="7">
-        <v>1.34</v>
-      </c>
-      <c r="AD18" s="7">
-        <f t="shared" si="10"/>
-        <v>1.93</v>
-      </c>
-      <c r="AE18" s="7">
-        <f t="shared" si="11"/>
-        <v>2.44</v>
-      </c>
-      <c r="AF18" s="7">
-        <f t="shared" si="12"/>
-        <v>1.29</v>
-      </c>
-      <c r="AG18" s="8">
-        <f t="shared" si="13"/>
-        <v>1.8</v>
-      </c>
-      <c r="AH18" s="7">
-        <v>0.24199999999999999</v>
-      </c>
-      <c r="AI18" s="27">
-        <v>3.4099999999999998E-2</v>
-      </c>
-      <c r="AJ18" s="7">
-        <v>0.41699999999999998</v>
-      </c>
-      <c r="AK18" s="7">
-        <v>0.14199999999999999</v>
-      </c>
-      <c r="AL18" s="9">
-        <f t="shared" si="14"/>
-        <v>0.83510000000000006</v>
-      </c>
-      <c r="AM18" s="7">
-        <v>0.88300000000000001</v>
-      </c>
-      <c r="AN18" s="7">
-        <v>0.23</v>
-      </c>
-      <c r="AO18" s="7">
-        <v>0.55200000000000005</v>
-      </c>
-      <c r="AP18" s="7">
-        <v>0.79700000000000004</v>
-      </c>
-    </row>
-    <row r="19" spans="1:42" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A19" s="22" t="s">
-        <v>41</v>
-      </c>
-      <c r="B19" s="8">
-        <v>0</v>
-      </c>
-      <c r="C19" s="20">
-        <v>0.09</v>
-      </c>
-      <c r="D19" s="7">
-        <v>1</v>
-      </c>
-      <c r="E19" s="7">
-        <v>2</v>
-      </c>
-      <c r="F19" s="8">
-        <v>5</v>
-      </c>
-      <c r="G19" s="20">
-        <v>0.2</v>
-      </c>
-      <c r="H19" s="7">
-        <v>0.5</v>
-      </c>
-      <c r="I19" s="7">
-        <v>1</v>
-      </c>
-      <c r="J19" s="8">
-        <v>1</v>
-      </c>
-      <c r="K19" s="7">
-        <v>2</v>
-      </c>
-      <c r="L19" s="7">
-        <v>2</v>
-      </c>
-      <c r="M19" s="8">
-        <v>2</v>
-      </c>
-      <c r="N19" s="7">
-        <v>2</v>
-      </c>
-      <c r="O19" s="7">
-        <v>3</v>
-      </c>
-      <c r="P19" s="8">
-        <v>2</v>
-      </c>
-      <c r="Q19" s="7">
-        <v>1</v>
-      </c>
-      <c r="R19" s="7">
-        <v>0.5</v>
-      </c>
-      <c r="S19" s="8">
-        <v>1</v>
-      </c>
-      <c r="V19" s="7">
-        <v>1.49</v>
-      </c>
-      <c r="W19" s="7">
-        <v>2.52</v>
-      </c>
-      <c r="X19" s="7">
-        <v>3.22</v>
-      </c>
-      <c r="Y19" s="7">
-        <v>3.04</v>
-      </c>
-      <c r="Z19" s="7">
-        <v>0.83699999999999997</v>
-      </c>
-      <c r="AA19" s="7">
-        <v>1.37</v>
-      </c>
-      <c r="AB19" s="7">
-        <v>1.79</v>
-      </c>
-      <c r="AC19" s="7">
-        <v>1.1200000000000001</v>
-      </c>
-      <c r="AD19" s="7">
-        <f t="shared" ref="AD19:AD22" si="15">V19-Z19-$T19</f>
-        <v>0.65300000000000002</v>
-      </c>
-      <c r="AE19" s="7">
-        <f t="shared" ref="AE19:AE22" si="16">W19-AA19-$T19</f>
-        <v>1.1499999999999999</v>
-      </c>
-      <c r="AF19" s="7">
-        <f t="shared" ref="AF19:AF22" si="17">X19-AB19-$U19</f>
-        <v>1.4300000000000002</v>
-      </c>
-      <c r="AG19" s="8">
-        <f t="shared" ref="AG19:AG22" si="18">Y19-AC19-$U19</f>
-        <v>1.92</v>
-      </c>
-      <c r="AH19" s="7">
-        <v>0.10299999999999999</v>
-      </c>
-      <c r="AI19" s="7">
-        <v>7.6700000000000004E-2</v>
-      </c>
-      <c r="AJ19" s="7">
-        <v>0.48299999999999998</v>
-      </c>
-      <c r="AK19" s="7">
-        <v>0.124</v>
-      </c>
-      <c r="AL19" s="9">
-        <f t="shared" ref="AL19:AL22" si="19">SUM(AH19:AK19)</f>
-        <v>0.78669999999999995</v>
-      </c>
-      <c r="AM19" s="7">
-        <v>0.95199999999999996</v>
-      </c>
-      <c r="AN19" s="7">
-        <v>0.24299999999999999</v>
-      </c>
-      <c r="AO19" s="7">
-        <v>0.156</v>
-      </c>
-      <c r="AP19" s="7">
-        <v>0.92900000000000005</v>
-      </c>
+      <c r="V18" s="7"/>
+      <c r="W18" s="7"/>
+      <c r="X18" s="7"/>
+      <c r="Y18" s="7"/>
+      <c r="Z18" s="7"/>
+      <c r="AA18" s="7"/>
+      <c r="AB18" s="7"/>
+      <c r="AC18" s="7"/>
+      <c r="AD18" s="7"/>
+      <c r="AE18" s="7"/>
+      <c r="AF18" s="7"/>
+      <c r="AG18" s="8"/>
+      <c r="AH18" s="7"/>
+      <c r="AI18" s="27"/>
+      <c r="AJ18" s="7"/>
+      <c r="AK18" s="7"/>
+      <c r="AL18" s="9"/>
+      <c r="AM18" s="7"/>
+      <c r="AN18" s="7"/>
+      <c r="AO18" s="7"/>
+      <c r="AP18" s="7"/>
+    </row>
+    <row r="19" spans="1:42" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="22"/>
+      <c r="B19" s="8"/>
+      <c r="C19" s="20"/>
+      <c r="F19" s="8"/>
+      <c r="G19" s="20"/>
+      <c r="J19" s="8"/>
+      <c r="M19" s="8"/>
+      <c r="P19" s="8"/>
+      <c r="S19" s="8"/>
+      <c r="AG19" s="8"/>
+      <c r="AL19" s="9"/>
     </row>
     <row r="20" spans="1:42" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="22"/>
-      <c r="B20" s="8">
-        <v>1</v>
-      </c>
+      <c r="B20" s="8"/>
       <c r="C20" s="20"/>
       <c r="D20" s="7"/>
       <c r="E20" s="7"/>
@@ -2802,207 +1323,44 @@
       <c r="S20" s="8"/>
       <c r="T20" s="7"/>
       <c r="U20" s="7"/>
-      <c r="V20" s="7">
-        <v>1.62</v>
-      </c>
-      <c r="W20" s="7">
-        <v>3.36</v>
-      </c>
-      <c r="X20" s="7">
-        <v>3.34</v>
-      </c>
-      <c r="Y20" s="7">
-        <v>3.11</v>
-      </c>
-      <c r="Z20" s="7">
-        <v>0</v>
-      </c>
-      <c r="AA20" s="7">
-        <v>1.24</v>
-      </c>
-      <c r="AB20" s="7">
-        <v>1.9</v>
-      </c>
-      <c r="AC20" s="7">
-        <v>1.7</v>
-      </c>
-      <c r="AD20" s="7">
-        <f t="shared" si="15"/>
-        <v>1.62</v>
-      </c>
-      <c r="AE20" s="7">
-        <f t="shared" si="16"/>
-        <v>2.12</v>
-      </c>
-      <c r="AF20" s="7">
-        <f t="shared" si="17"/>
-        <v>1.44</v>
-      </c>
-      <c r="AG20" s="8">
-        <f t="shared" si="18"/>
-        <v>1.41</v>
-      </c>
-      <c r="AH20" s="7">
-        <v>9.7000000000000003E-2</v>
-      </c>
-      <c r="AI20" s="27">
-        <v>4.0300000000000002E-2</v>
-      </c>
-      <c r="AJ20" s="7">
-        <v>0.46200000000000002</v>
-      </c>
-      <c r="AK20" s="7">
-        <v>0.14099999999999999</v>
-      </c>
-      <c r="AL20" s="9">
-        <f t="shared" si="19"/>
-        <v>0.74030000000000007</v>
-      </c>
-      <c r="AM20" s="7">
-        <v>0.879</v>
-      </c>
-      <c r="AN20" s="7">
-        <v>0.215</v>
-      </c>
-      <c r="AO20" s="7">
-        <v>0.24299999999999999</v>
-      </c>
-      <c r="AP20" s="7">
-        <v>0.93799999999999994</v>
-      </c>
+      <c r="V20" s="7"/>
+      <c r="W20" s="7"/>
+      <c r="X20" s="7"/>
+      <c r="Y20" s="7"/>
+      <c r="Z20" s="7"/>
+      <c r="AA20" s="7"/>
+      <c r="AB20" s="7"/>
+      <c r="AC20" s="7"/>
+      <c r="AD20" s="7"/>
+      <c r="AE20" s="7"/>
+      <c r="AF20" s="7"/>
+      <c r="AG20" s="8"/>
+      <c r="AH20" s="7"/>
+      <c r="AI20" s="27"/>
+      <c r="AJ20" s="7"/>
+      <c r="AK20" s="7"/>
+      <c r="AL20" s="9"/>
+      <c r="AM20" s="7"/>
+      <c r="AN20" s="7"/>
+      <c r="AO20" s="7"/>
+      <c r="AP20" s="7"/>
     </row>
     <row r="21" spans="1:42" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="22" t="s">
-        <v>37</v>
-      </c>
-      <c r="B21" s="8">
-        <v>0</v>
-      </c>
-      <c r="C21" s="20">
-        <v>0.5</v>
-      </c>
-      <c r="D21" s="7">
-        <v>-1</v>
-      </c>
-      <c r="E21" s="7">
-        <v>1</v>
-      </c>
-      <c r="F21" s="8">
-        <v>0</v>
-      </c>
-      <c r="G21" s="20">
-        <v>0.5</v>
-      </c>
-      <c r="H21" s="7">
-        <v>-1</v>
-      </c>
-      <c r="I21" s="7">
-        <v>1</v>
-      </c>
-      <c r="J21" s="8">
-        <v>0</v>
-      </c>
-      <c r="K21" s="7">
-        <v>2</v>
-      </c>
-      <c r="L21" s="7">
-        <v>2</v>
-      </c>
-      <c r="M21" s="8">
-        <v>2</v>
-      </c>
-      <c r="N21" s="7">
-        <v>1</v>
-      </c>
-      <c r="O21" s="7">
-        <v>1</v>
-      </c>
-      <c r="P21" s="8">
-        <v>1</v>
-      </c>
-      <c r="Q21" s="7">
-        <v>1</v>
-      </c>
-      <c r="R21" s="7">
-        <v>1</v>
-      </c>
-      <c r="S21" s="8">
-        <v>1</v>
-      </c>
-      <c r="V21" s="7">
-        <v>2.96</v>
-      </c>
-      <c r="W21" s="7">
-        <v>2.96</v>
-      </c>
-      <c r="X21" s="7">
-        <v>2.96</v>
-      </c>
-      <c r="Y21" s="7">
-        <v>2.96</v>
-      </c>
-      <c r="Z21" s="7">
-        <v>1.52</v>
-      </c>
-      <c r="AA21" s="7">
-        <v>1.52</v>
-      </c>
-      <c r="AB21" s="7">
-        <v>1.52</v>
-      </c>
-      <c r="AC21" s="7">
-        <v>1.52</v>
-      </c>
-      <c r="AD21" s="7">
-        <f t="shared" si="15"/>
-        <v>1.44</v>
-      </c>
-      <c r="AE21" s="7">
-        <f t="shared" si="16"/>
-        <v>1.44</v>
-      </c>
-      <c r="AF21" s="7">
-        <f t="shared" si="17"/>
-        <v>1.44</v>
-      </c>
-      <c r="AG21" s="8">
-        <f t="shared" si="18"/>
-        <v>1.44</v>
-      </c>
-      <c r="AH21" s="7">
-        <v>0.152</v>
-      </c>
-      <c r="AI21" s="7">
-        <v>0.152</v>
-      </c>
-      <c r="AJ21" s="7">
-        <v>0.152</v>
-      </c>
-      <c r="AK21" s="7">
-        <v>0.152</v>
-      </c>
-      <c r="AL21" s="9">
-        <f t="shared" si="19"/>
-        <v>0.60799999999999998</v>
-      </c>
-      <c r="AM21" s="7">
-        <v>0.46100000000000002</v>
-      </c>
-      <c r="AN21" s="7">
-        <v>0.46100000000000002</v>
-      </c>
-      <c r="AO21" s="7">
-        <v>0.435</v>
-      </c>
-      <c r="AP21" s="7">
-        <v>0.435</v>
-      </c>
+      <c r="A21" s="22"/>
+      <c r="B21" s="8"/>
+      <c r="C21" s="20"/>
+      <c r="F21" s="8"/>
+      <c r="G21" s="20"/>
+      <c r="J21" s="8"/>
+      <c r="M21" s="8"/>
+      <c r="P21" s="8"/>
+      <c r="S21" s="8"/>
+      <c r="AG21" s="8"/>
+      <c r="AL21" s="9"/>
     </row>
     <row r="22" spans="1:42" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="22"/>
-      <c r="B22" s="8">
-        <v>1</v>
-      </c>
+      <c r="B22" s="8"/>
       <c r="C22" s="20"/>
       <c r="F22" s="8"/>
       <c r="G22" s="20"/>
@@ -3010,207 +1368,25 @@
       <c r="M22" s="8"/>
       <c r="P22" s="8"/>
       <c r="S22" s="8"/>
-      <c r="V22" s="7">
-        <v>2.0299999999999998</v>
-      </c>
-      <c r="W22" s="7">
-        <v>3.32</v>
-      </c>
-      <c r="X22" s="7">
-        <v>3.29</v>
-      </c>
-      <c r="Y22" s="7">
-        <v>2.81</v>
-      </c>
-      <c r="Z22" s="7">
-        <v>0</v>
-      </c>
-      <c r="AA22" s="7">
-        <v>1.29</v>
-      </c>
-      <c r="AB22" s="7">
-        <v>1.96</v>
-      </c>
-      <c r="AC22" s="7">
-        <v>1.49</v>
-      </c>
-      <c r="AD22" s="7">
-        <f t="shared" si="15"/>
-        <v>2.0299999999999998</v>
-      </c>
-      <c r="AE22" s="7">
-        <f t="shared" si="16"/>
-        <v>2.0299999999999998</v>
-      </c>
-      <c r="AF22" s="7">
-        <f t="shared" si="17"/>
-        <v>1.33</v>
-      </c>
-      <c r="AG22" s="8">
-        <f t="shared" si="18"/>
-        <v>1.32</v>
-      </c>
-      <c r="AH22" s="7">
-        <v>0.32700000000000001</v>
-      </c>
-      <c r="AI22" s="7">
-        <v>9.0499999999999997E-2</v>
-      </c>
-      <c r="AJ22" s="7">
-        <v>9.3600000000000003E-2</v>
-      </c>
-      <c r="AK22" s="7">
-        <v>0.15</v>
-      </c>
-      <c r="AL22" s="9">
-        <f t="shared" si="19"/>
-        <v>0.66110000000000002</v>
-      </c>
-      <c r="AM22" s="7">
-        <v>0.184</v>
-      </c>
-      <c r="AN22" s="7">
-        <v>0.34</v>
-      </c>
-      <c r="AO22" s="7">
-        <v>0.84899999999999998</v>
-      </c>
-      <c r="AP22" s="7">
-        <v>0.32300000000000001</v>
-      </c>
-    </row>
-    <row r="23" spans="1:42" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A23" s="22" t="s">
-        <v>42</v>
-      </c>
-      <c r="B23" s="8">
-        <v>0</v>
-      </c>
-      <c r="C23" s="20">
-        <v>0.5</v>
-      </c>
-      <c r="D23" s="7">
-        <v>-1</v>
-      </c>
-      <c r="E23" s="7">
-        <v>1</v>
-      </c>
-      <c r="F23" s="8">
-        <v>1</v>
-      </c>
-      <c r="G23" s="20">
-        <v>0.5</v>
-      </c>
-      <c r="H23" s="7">
-        <v>-1</v>
-      </c>
-      <c r="I23" s="7">
-        <v>1</v>
-      </c>
-      <c r="J23" s="8">
-        <v>1</v>
-      </c>
-      <c r="K23" s="7">
-        <v>2</v>
-      </c>
-      <c r="L23" s="7">
-        <v>2</v>
-      </c>
-      <c r="M23" s="8">
-        <v>2</v>
-      </c>
-      <c r="N23" s="7">
-        <v>1</v>
-      </c>
-      <c r="O23" s="7">
-        <v>1</v>
-      </c>
-      <c r="P23" s="8">
-        <v>1</v>
-      </c>
-      <c r="Q23" s="7">
-        <v>1</v>
-      </c>
-      <c r="R23" s="7">
-        <v>1</v>
-      </c>
-      <c r="S23" s="8">
-        <v>1</v>
-      </c>
-      <c r="V23" s="7">
-        <v>2.89</v>
-      </c>
-      <c r="W23" s="7">
-        <v>2.89</v>
-      </c>
-      <c r="X23" s="7">
-        <v>3.39</v>
-      </c>
-      <c r="Y23" s="7">
-        <v>3.39</v>
-      </c>
-      <c r="Z23" s="7">
-        <v>1.54</v>
-      </c>
-      <c r="AA23" s="7">
-        <v>1.54</v>
-      </c>
-      <c r="AB23" s="7">
-        <v>1.65</v>
-      </c>
-      <c r="AC23" s="7">
-        <v>1.65</v>
-      </c>
-      <c r="AD23" s="7">
-        <f t="shared" ref="AD23:AD24" si="20">V23-Z23-$T23</f>
-        <v>1.35</v>
-      </c>
-      <c r="AE23" s="7">
-        <f t="shared" ref="AE23:AE24" si="21">W23-AA23-$T23</f>
-        <v>1.35</v>
-      </c>
-      <c r="AF23" s="7">
-        <f t="shared" ref="AF23:AF24" si="22">X23-AB23-$U23</f>
-        <v>1.7400000000000002</v>
-      </c>
-      <c r="AG23" s="8">
-        <f t="shared" ref="AG23:AG24" si="23">Y23-AC23-$U23</f>
-        <v>1.7400000000000002</v>
-      </c>
-      <c r="AH23" s="7">
-        <v>0.13</v>
-      </c>
-      <c r="AI23" s="7">
-        <v>0.13</v>
-      </c>
-      <c r="AJ23" s="7">
-        <v>0.21299999999999999</v>
-      </c>
-      <c r="AK23" s="7">
-        <v>0.21299999999999999</v>
-      </c>
-      <c r="AL23" s="9">
-        <f t="shared" ref="AL23:AL24" si="24">SUM(AH23:AK23)</f>
-        <v>0.68599999999999994</v>
-      </c>
-      <c r="AM23" s="7">
-        <v>0.55100000000000005</v>
-      </c>
-      <c r="AN23" s="7">
-        <v>0.55100000000000005</v>
-      </c>
-      <c r="AO23" s="7">
-        <v>0.33</v>
-      </c>
-      <c r="AP23" s="7">
-        <v>0.74099999999999999</v>
-      </c>
+      <c r="AG22" s="8"/>
+      <c r="AL22" s="9"/>
+    </row>
+    <row r="23" spans="1:42" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="22"/>
+      <c r="B23" s="8"/>
+      <c r="C23" s="20"/>
+      <c r="F23" s="8"/>
+      <c r="G23" s="20"/>
+      <c r="J23" s="8"/>
+      <c r="M23" s="8"/>
+      <c r="P23" s="8"/>
+      <c r="S23" s="8"/>
+      <c r="AG23" s="8"/>
+      <c r="AL23" s="9"/>
     </row>
     <row r="24" spans="1:42" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="22"/>
-      <c r="B24" s="8">
-        <v>1</v>
-      </c>
+      <c r="B24" s="8"/>
       <c r="C24" s="20"/>
       <c r="F24" s="8"/>
       <c r="G24" s="20"/>
@@ -3218,207 +1394,25 @@
       <c r="M24" s="8"/>
       <c r="P24" s="8"/>
       <c r="S24" s="8"/>
-      <c r="V24" s="7">
-        <v>2.0099999999999998</v>
-      </c>
-      <c r="W24" s="7">
-        <v>3.33</v>
-      </c>
-      <c r="X24" s="7">
-        <v>3.55</v>
-      </c>
-      <c r="Y24" s="7">
-        <v>3.26</v>
-      </c>
-      <c r="Z24" s="7">
-        <v>0</v>
-      </c>
-      <c r="AA24" s="7">
-        <v>1.32</v>
-      </c>
-      <c r="AB24" s="7">
-        <v>1.95</v>
-      </c>
-      <c r="AC24" s="7">
-        <v>1.66</v>
-      </c>
-      <c r="AD24" s="7">
-        <f t="shared" si="20"/>
-        <v>2.0099999999999998</v>
-      </c>
-      <c r="AE24" s="7">
-        <f t="shared" si="21"/>
-        <v>2.0099999999999998</v>
-      </c>
-      <c r="AF24" s="7">
-        <f t="shared" si="22"/>
-        <v>1.5999999999999999</v>
-      </c>
-      <c r="AG24" s="8">
-        <f t="shared" si="23"/>
-        <v>1.5999999999999999</v>
-      </c>
-      <c r="AH24" s="7">
-        <v>0.27400000000000002</v>
-      </c>
-      <c r="AI24" s="7">
-        <v>7.3200000000000001E-2</v>
-      </c>
-      <c r="AJ24" s="7">
-        <v>0.161</v>
-      </c>
-      <c r="AK24" s="7">
-        <v>0.214</v>
-      </c>
-      <c r="AL24" s="9">
-        <f t="shared" si="24"/>
-        <v>0.72219999999999995</v>
-      </c>
-      <c r="AM24" s="7">
-        <v>0.313</v>
-      </c>
-      <c r="AN24" s="7">
-        <v>0.45200000000000001</v>
-      </c>
-      <c r="AO24" s="7">
-        <v>0.69899999999999995</v>
-      </c>
-      <c r="AP24" s="7">
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="25" spans="1:42" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A25" s="22" t="s">
-        <v>43</v>
-      </c>
-      <c r="B25" s="8">
-        <v>0</v>
-      </c>
-      <c r="C25" s="20">
-        <v>0.5</v>
-      </c>
-      <c r="D25" s="7">
-        <v>-1</v>
-      </c>
-      <c r="E25" s="7">
-        <v>1</v>
-      </c>
-      <c r="F25" s="8">
-        <v>-1</v>
-      </c>
-      <c r="G25" s="20">
-        <v>0.5</v>
-      </c>
-      <c r="H25" s="7">
-        <v>-1</v>
-      </c>
-      <c r="I25" s="7">
-        <v>1</v>
-      </c>
-      <c r="J25" s="8">
-        <v>-1</v>
-      </c>
-      <c r="K25" s="7">
-        <v>2</v>
-      </c>
-      <c r="L25" s="7">
-        <v>2</v>
-      </c>
-      <c r="M25" s="8">
-        <v>2</v>
-      </c>
-      <c r="N25" s="7">
-        <v>1</v>
-      </c>
-      <c r="O25" s="7">
-        <v>1</v>
-      </c>
-      <c r="P25" s="8">
-        <v>1</v>
-      </c>
-      <c r="Q25" s="7">
-        <v>1</v>
-      </c>
-      <c r="R25" s="7">
-        <v>1</v>
-      </c>
-      <c r="S25" s="8">
-        <v>1</v>
-      </c>
-      <c r="V25" s="7">
-        <v>3.02</v>
-      </c>
-      <c r="W25" s="7">
-        <v>3.02</v>
-      </c>
-      <c r="X25" s="7">
-        <v>2.62</v>
-      </c>
-      <c r="Y25" s="7">
-        <v>2.62</v>
-      </c>
-      <c r="Z25" s="7">
-        <v>1.5</v>
-      </c>
-      <c r="AA25" s="7">
-        <v>1.5</v>
-      </c>
-      <c r="AB25" s="7">
-        <v>1.39</v>
-      </c>
-      <c r="AC25" s="7">
-        <v>1.39</v>
-      </c>
-      <c r="AD25" s="7">
-        <f t="shared" ref="AD25:AD26" si="25">V25-Z25-$T25</f>
-        <v>1.52</v>
-      </c>
-      <c r="AE25" s="7">
-        <f t="shared" ref="AE25:AE26" si="26">W25-AA25-$T25</f>
-        <v>1.52</v>
-      </c>
-      <c r="AF25" s="7">
-        <f t="shared" ref="AF25:AF26" si="27">X25-AB25-$U25</f>
-        <v>1.2300000000000002</v>
-      </c>
-      <c r="AG25" s="8">
-        <f t="shared" ref="AG25:AG26" si="28">Y25-AC25-$U25</f>
-        <v>1.2300000000000002</v>
-      </c>
-      <c r="AH25" s="7">
-        <v>0.17100000000000001</v>
-      </c>
-      <c r="AI25" s="7">
-        <v>0.17100000000000001</v>
-      </c>
-      <c r="AJ25" s="7">
-        <v>9.3399999999999997E-2</v>
-      </c>
-      <c r="AK25" s="7">
-        <v>9.3399999999999997E-2</v>
-      </c>
-      <c r="AL25" s="9">
-        <f t="shared" ref="AL25:AL26" si="29">SUM(AH25:AK25)</f>
-        <v>0.52880000000000005</v>
-      </c>
-      <c r="AM25" s="7">
-        <v>0.38600000000000001</v>
-      </c>
-      <c r="AN25" s="7">
-        <v>0.38600000000000001</v>
-      </c>
-      <c r="AO25" s="7">
-        <v>0.51800000000000002</v>
-      </c>
-      <c r="AP25" s="7">
-        <v>0.23</v>
-      </c>
+      <c r="AG24" s="8"/>
+      <c r="AL24" s="9"/>
+    </row>
+    <row r="25" spans="1:42" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="22"/>
+      <c r="B25" s="8"/>
+      <c r="C25" s="20"/>
+      <c r="F25" s="8"/>
+      <c r="G25" s="20"/>
+      <c r="J25" s="8"/>
+      <c r="M25" s="8"/>
+      <c r="P25" s="8"/>
+      <c r="S25" s="8"/>
+      <c r="AG25" s="8"/>
+      <c r="AL25" s="9"/>
     </row>
     <row r="26" spans="1:42" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="22"/>
-      <c r="B26" s="8">
-        <v>1</v>
-      </c>
+      <c r="B26" s="8"/>
       <c r="C26" s="20"/>
       <c r="F26" s="8"/>
       <c r="G26" s="20"/>
@@ -3426,74 +1420,8 @@
       <c r="M26" s="8"/>
       <c r="P26" s="8"/>
       <c r="S26" s="8"/>
-      <c r="V26" s="7">
-        <v>2.0699999999999998</v>
-      </c>
-      <c r="W26" s="7">
-        <v>3.32</v>
-      </c>
-      <c r="X26" s="7">
-        <v>3.17</v>
-      </c>
-      <c r="Y26" s="7">
-        <v>2.4700000000000002</v>
-      </c>
-      <c r="Z26" s="7">
-        <v>0</v>
-      </c>
-      <c r="AA26" s="7">
-        <v>1.25</v>
-      </c>
-      <c r="AB26" s="7">
-        <v>2.0099999999999998</v>
-      </c>
-      <c r="AC26" s="7">
-        <v>1.31</v>
-      </c>
-      <c r="AD26" s="7">
-        <f t="shared" si="25"/>
-        <v>2.0699999999999998</v>
-      </c>
-      <c r="AE26" s="7">
-        <f t="shared" si="26"/>
-        <v>2.0699999999999998</v>
-      </c>
-      <c r="AF26" s="7">
-        <f t="shared" si="27"/>
-        <v>1.1600000000000001</v>
-      </c>
-      <c r="AG26" s="8">
-        <f t="shared" si="28"/>
-        <v>1.1600000000000001</v>
-      </c>
-      <c r="AH26" s="7">
-        <v>0.36699999999999999</v>
-      </c>
-      <c r="AI26" s="7">
-        <v>0.106</v>
-      </c>
-      <c r="AJ26" s="7">
-        <v>4.4900000000000002E-2</v>
-      </c>
-      <c r="AK26" s="7">
-        <v>9.0300000000000005E-2</v>
-      </c>
-      <c r="AL26" s="9">
-        <f t="shared" si="29"/>
-        <v>0.60820000000000007</v>
-      </c>
-      <c r="AM26" s="7">
-        <v>9.0399999999999994E-2</v>
-      </c>
-      <c r="AN26" s="7">
-        <v>0.25</v>
-      </c>
-      <c r="AO26" s="7">
-        <v>0.97599999999999998</v>
-      </c>
-      <c r="AP26" s="7">
-        <v>0.156</v>
-      </c>
+      <c r="AG26" s="8"/>
+      <c r="AL26" s="9"/>
     </row>
     <row r="27" spans="1:42" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="23"/>

</xml_diff>